<commit_message>
Update missing fields under timestamp column
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E43600-D06B-5943-84CA-4C67E742EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="8700" yWindow="3060" windowWidth="20100" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -36,14 +45,16 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.spsnational.org/about/governance/zones</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t>)</t>
@@ -85,28 +96,32 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>email1@mail.edu</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">; </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>email2@mail.edu</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t>)</t>
@@ -118,9 +133,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.spsnational.org/about/governance/national-council/nominations-elections</t>
     </r>
@@ -143,9 +159,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>www.spsnational.org/code-conduct</t>
     </r>
@@ -156,9 +173,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.sigmapisigma.org/congress/2022</t>
     </r>
@@ -193,14 +211,16 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>www.spsnational.org</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> website?</t>
@@ -212,14 +232,16 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>www.spsnational.org</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> website? </t>
@@ -234,9 +256,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>www.spsnational.org/about/governance/sps-information-handbook</t>
     </r>
@@ -247,9 +270,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.sigmapisigma.org/sigmapisigma/pion-resources</t>
     </r>
@@ -260,23 +284,26 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.spsnational.org/awards/service</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://www.sigmapisigma.org/sigmapisigma/awards/outstanding-service</t>
     </r>
@@ -287,9 +314,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>www.spsnational.org/careerstoolbox</t>
     </r>
@@ -315,9 +343,10 @@
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
       </rPr>
       <t>https://rb.gy/atr9rp</t>
     </r>
@@ -1091,35 +1120,47 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1127,57 +1168,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1367,30 +1402,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="22.88"/>
-    <col customWidth="1" min="3" max="3" width="23.75"/>
-    <col customWidth="1" min="4" max="4" width="22.63"/>
-    <col customWidth="1" min="7" max="7" width="8.63"/>
-    <col customWidth="1" min="14" max="14" width="19.88"/>
-    <col customWidth="1" min="46" max="46" width="24.0"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" customWidth="1"/>
+    <col min="46" max="46" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1528,7 +1568,7 @@
       <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AV1" s="1"/>
@@ -1538,9 +1578,9 @@
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>45448.510233657405</v>
+    <row r="2" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7">
+        <v>45448.510231481479</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>47</v>
@@ -1557,10 +1597,10 @@
       <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>50</v>
       </c>
       <c r="I2" s="1"/>
@@ -1594,8 +1634,8 @@
       <c r="Y2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" s="5">
-        <v>20.0</v>
+      <c r="Z2" s="3">
+        <v>20</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>55</v>
@@ -1637,17 +1677,17 @@
       <c r="AP2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AT2" s="7" t="s">
+      <c r="AT2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AU2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AV2" s="1"/>
@@ -1657,9 +1697,9 @@
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" s="4">
-        <v>45455.84625959491</v>
+    <row r="3" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="7">
+        <v>45455.846261574072</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>64</v>
@@ -1676,19 +1716,19 @@
       <c r="F3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="5">
-        <v>1.0</v>
+      <c r="G3" s="3">
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="1" t="s">
         <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1733,8 +1773,8 @@
       <c r="Y3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z3" s="5">
-        <v>30.0</v>
+      <c r="Z3" s="3">
+        <v>30</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>51</v>
@@ -1744,8 +1784,8 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="5">
-        <v>4.0</v>
+      <c r="AG3" s="3">
+        <v>4</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>51</v>
@@ -1779,10 +1819,10 @@
       <c r="AS3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AT3" s="7" t="s">
+      <c r="AT3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AU3" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AV3" s="1"/>
@@ -1792,14 +1832,14 @@
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" s="4">
-        <v>45458.85255541667</v>
+    <row r="4" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="7">
+        <v>45458.85255787037</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="1"/>
@@ -1809,10 +1849,10 @@
       <c r="F4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1860,8 +1900,8 @@
       <c r="Y4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z4" s="5">
-        <v>150.0</v>
+      <c r="Z4" s="3">
+        <v>150</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>51</v>
@@ -1874,7 +1914,7 @@
         <v>55</v>
       </c>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="3" t="s">
+      <c r="AF4" s="1" t="s">
         <v>98</v>
       </c>
       <c r="AG4" s="1"/>
@@ -1901,17 +1941,17 @@
       <c r="AP4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>99</v>
       </c>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AT4" s="7" t="s">
+      <c r="AT4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AU4" s="3" t="s">
+      <c r="AU4" s="1" t="s">
         <v>102</v>
       </c>
       <c r="AV4" s="1"/>
@@ -1921,9 +1961,9 @@
       <c r="AZ4" s="1"/>
       <c r="BA4" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" s="4">
-        <v>45457.86581069445</v>
+    <row r="5" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="7">
+        <v>45457.865810185183</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>103</v>
@@ -1938,10 +1978,10 @@
       <c r="F5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>107</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1995,8 +2035,8 @@
       <c r="Y5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="5">
-        <v>100.0</v>
+      <c r="Z5" s="3">
+        <v>100</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>55</v>
@@ -2049,10 +2089,10 @@
       <c r="AS5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AT5" s="7" t="s">
+      <c r="AT5" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="AU5" s="3" t="s">
+      <c r="AU5" s="1" t="s">
         <v>128</v>
       </c>
       <c r="AV5" s="1"/>
@@ -2062,9 +2102,9 @@
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
     </row>
-    <row r="6">
-      <c r="A6" s="4">
-        <v>45455.72483760417</v>
+    <row r="6" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>45455.72483796296</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>129</v>
@@ -2079,10 +2119,10 @@
       <c r="F6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>132</v>
       </c>
       <c r="I6" s="1"/>
@@ -2116,8 +2156,8 @@
       <c r="Y6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z6" s="5">
-        <v>14.0</v>
+      <c r="Z6" s="3">
+        <v>14</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>55</v>
@@ -2138,7 +2178,7 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
-      <c r="AP6" s="3" t="s">
+      <c r="AP6" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AQ6" s="1"/>
@@ -2146,7 +2186,7 @@
       <c r="AS6" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AT6" s="6" t="s">
+      <c r="AT6" s="4" t="s">
         <v>136</v>
       </c>
       <c r="AU6" s="1"/>
@@ -2157,9 +2197,9 @@
       <c r="AZ6" s="1"/>
       <c r="BA6" s="1"/>
     </row>
-    <row r="7">
-      <c r="A7" s="4">
-        <v>45457.566966238424</v>
+    <row r="7" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>45457.566967592589</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>137</v>
@@ -2167,7 +2207,7 @@
       <c r="C7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2176,8 +2216,8 @@
       <c r="F7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="5">
-        <v>1.0</v>
+      <c r="G7" s="3">
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>141</v>
@@ -2213,8 +2253,8 @@
       <c r="Y7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z7" s="5">
-        <v>20.0</v>
+      <c r="Z7" s="3">
+        <v>20</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>55</v>
@@ -2234,8 +2274,8 @@
       <c r="AF7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AG7" s="5">
-        <v>1.0</v>
+      <c r="AG7" s="3">
+        <v>1</v>
       </c>
       <c r="AH7" s="1" t="s">
         <v>55</v>
@@ -2271,7 +2311,7 @@
       <c r="AS7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AT7" s="6" t="s">
+      <c r="AT7" s="4" t="s">
         <v>151</v>
       </c>
       <c r="AU7" s="1"/>
@@ -2282,9 +2322,9 @@
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
     </row>
-    <row r="8">
-      <c r="A8" s="4">
-        <v>45457.48966746528</v>
+    <row r="8" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="7">
+        <v>45457.489664351851</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>152</v>
@@ -2299,8 +2339,8 @@
       <c r="F8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G8" s="5">
-        <v>1.0</v>
+      <c r="G8" s="3">
+        <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>156</v>
@@ -2356,8 +2396,8 @@
       <c r="Y8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z8" s="5">
-        <v>30.0</v>
+      <c r="Z8" s="3">
+        <v>30</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>51</v>
@@ -2396,7 +2436,7 @@
         <v>55</v>
       </c>
       <c r="AO8" s="1"/>
-      <c r="AP8" s="3" t="s">
+      <c r="AP8" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AQ8" s="1"/>
@@ -2406,10 +2446,10 @@
       <c r="AS8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AT8" s="7" t="s">
+      <c r="AT8" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="AU8" s="3" t="s">
+      <c r="AU8" s="1" t="s">
         <v>174</v>
       </c>
       <c r="AV8" s="1"/>
@@ -2419,9 +2459,9 @@
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
     </row>
-    <row r="9">
-      <c r="A9" s="4">
-        <v>45411.40461200231</v>
+    <row r="9" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="7">
+        <v>45411.404606481483</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>175</v>
@@ -2436,8 +2476,8 @@
       <c r="F9" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="5">
-        <v>1.0</v>
+      <c r="G9" s="3">
+        <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>179</v>
@@ -2463,7 +2503,7 @@
       <c r="O9" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="1" t="s">
         <v>187</v>
       </c>
       <c r="Q9" s="1"/>
@@ -2489,8 +2529,8 @@
       <c r="Y9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z9" s="5">
-        <v>20.0</v>
+      <c r="Z9" s="3">
+        <v>20</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>51</v>
@@ -2506,8 +2546,8 @@
       <c r="AF9" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AG9" s="5">
-        <v>1.0</v>
+      <c r="AG9" s="3">
+        <v>1</v>
       </c>
       <c r="AH9" s="1" t="s">
         <v>51</v>
@@ -2534,7 +2574,7 @@
       <c r="AP9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AQ9" s="3" t="s">
+      <c r="AQ9" s="1" t="s">
         <v>192</v>
       </c>
       <c r="AR9" s="1"/>
@@ -2548,9 +2588,9 @@
       <c r="AZ9" s="1"/>
       <c r="BA9" s="1"/>
     </row>
-    <row r="10">
-      <c r="A10" s="4">
-        <v>45447.74182239584</v>
+    <row r="10" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>45447.74181712963</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>193</v>
@@ -2565,10 +2605,10 @@
       <c r="F10" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G10" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -2622,8 +2662,8 @@
       <c r="Y10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z10" s="5">
-        <v>48.0</v>
+      <c r="Z10" s="3">
+        <v>48</v>
       </c>
       <c r="AA10" s="1" t="s">
         <v>55</v>
@@ -2639,8 +2679,8 @@
       <c r="AF10" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="AG10" s="5">
-        <v>5.0</v>
+      <c r="AG10" s="3">
+        <v>5</v>
       </c>
       <c r="AH10" s="1" t="s">
         <v>51</v>
@@ -2674,10 +2714,10 @@
       <c r="AS10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AT10" s="7" t="s">
+      <c r="AT10" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="AU10" s="3" t="s">
+      <c r="AU10" s="1" t="s">
         <v>215</v>
       </c>
       <c r="AV10" s="1"/>
@@ -2687,14 +2727,14 @@
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="4">
-        <v>45450.921952442135</v>
+    <row r="11" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>45450.921956018516</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>217</v>
       </c>
       <c r="D11" s="1"/>
@@ -2704,10 +2744,10 @@
       <c r="F11" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G11" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>220</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -2761,8 +2801,8 @@
       <c r="Y11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z11" s="5">
-        <v>75.0</v>
+      <c r="Z11" s="3">
+        <v>75</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>51</v>
@@ -2780,8 +2820,8 @@
       <c r="AF11" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AG11" s="5">
-        <v>1.0</v>
+      <c r="AG11" s="3">
+        <v>1</v>
       </c>
       <c r="AH11" s="1" t="s">
         <v>55</v>
@@ -2815,10 +2855,10 @@
       <c r="AS11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AT11" s="7" t="s">
+      <c r="AT11" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="AU11" s="3" t="s">
+      <c r="AU11" s="1" t="s">
         <v>238</v>
       </c>
       <c r="AV11" s="1"/>
@@ -2828,9 +2868,9 @@
       <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
     </row>
-    <row r="12">
-      <c r="A12" s="4">
-        <v>45465.165206805555</v>
+    <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>45465.165208333332</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>239</v>
@@ -2847,10 +2887,10 @@
       <c r="F12" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="G12" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>243</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2904,8 +2944,8 @@
       <c r="Y12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z12" s="5">
-        <v>60.0</v>
+      <c r="Z12" s="3">
+        <v>60</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>55</v>
@@ -2925,8 +2965,8 @@
       <c r="AF12" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="AG12" s="5">
-        <v>2.0</v>
+      <c r="AG12" s="3">
+        <v>2</v>
       </c>
       <c r="AH12" s="1" t="s">
         <v>51</v>
@@ -2960,7 +3000,7 @@
       <c r="AS12" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AT12" s="6" t="s">
+      <c r="AT12" s="4" t="s">
         <v>258</v>
       </c>
       <c r="AU12" s="1"/>
@@ -2971,14 +3011,14 @@
       <c r="AZ12" s="1"/>
       <c r="BA12" s="1"/>
     </row>
-    <row r="13">
-      <c r="A13" s="4">
-        <v>45454.738026226856</v>
+    <row r="13" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>45454.738020833334</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="1"/>
@@ -2988,8 +3028,8 @@
       <c r="F13" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G13" s="5">
-        <v>1.0</v>
+      <c r="G13" s="3">
+        <v>1</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
@@ -3043,8 +3083,8 @@
       <c r="Y13" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Z13" s="5">
-        <v>20.0</v>
+      <c r="Z13" s="3">
+        <v>20</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>55</v>
@@ -3060,8 +3100,8 @@
       <c r="AF13" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AG13" s="5">
-        <v>1.0</v>
+      <c r="AG13" s="3">
+        <v>1</v>
       </c>
       <c r="AH13" s="1" t="s">
         <v>51</v>
@@ -3086,17 +3126,17 @@
       <c r="AP13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AQ13" s="3" t="s">
+      <c r="AQ13" s="1" t="s">
         <v>276</v>
       </c>
       <c r="AR13" s="1"/>
       <c r="AS13" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="AT13" s="7" t="s">
+      <c r="AT13" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="AU13" s="3" t="s">
+      <c r="AU13" s="1" t="s">
         <v>279</v>
       </c>
       <c r="AV13" s="1"/>
@@ -3106,9 +3146,9 @@
       <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
     </row>
-    <row r="14">
-      <c r="A14" s="4">
-        <v>45450.969664641205</v>
+    <row r="14" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="7">
+        <v>45450.969664351855</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>280</v>
@@ -3125,8 +3165,8 @@
       <c r="F14" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G14" s="5">
-        <v>1.0</v>
+      <c r="G14" s="3">
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>285</v>
@@ -3182,8 +3222,8 @@
       <c r="Y14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z14" s="5">
-        <v>32.0</v>
+      <c r="Z14" s="3">
+        <v>32</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>51</v>
@@ -3201,8 +3241,8 @@
       <c r="AF14" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="AG14" s="5">
-        <v>2.0</v>
+      <c r="AG14" s="3">
+        <v>2</v>
       </c>
       <c r="AH14" s="1" t="s">
         <v>51</v>
@@ -3224,7 +3264,7 @@
         <v>55</v>
       </c>
       <c r="AO14" s="1"/>
-      <c r="AP14" s="3" t="s">
+      <c r="AP14" s="1" t="s">
         <v>297</v>
       </c>
       <c r="AQ14" s="1"/>
@@ -3232,10 +3272,10 @@
       <c r="AS14" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AT14" s="7" t="s">
+      <c r="AT14" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="AU14" s="3" t="s">
+      <c r="AU14" s="1" t="s">
         <v>300</v>
       </c>
       <c r="AV14" s="1"/>
@@ -3247,38 +3287,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G1"/>
-    <hyperlink r:id="rId2" ref="R1"/>
-    <hyperlink r:id="rId3" ref="S1"/>
-    <hyperlink r:id="rId4" ref="X1"/>
-    <hyperlink r:id="rId5" ref="Y1"/>
-    <hyperlink r:id="rId6" ref="AH1"/>
-    <hyperlink r:id="rId7" ref="AI1"/>
-    <hyperlink r:id="rId8" ref="AK1"/>
-    <hyperlink r:id="rId9" ref="AL1"/>
-    <hyperlink r:id="rId10" ref="AM1"/>
-    <hyperlink r:id="rId11" ref="AN1"/>
-    <hyperlink r:id="rId12" ref="AT1"/>
-    <hyperlink r:id="rId13" ref="H2"/>
-    <hyperlink r:id="rId14" ref="AT2"/>
-    <hyperlink r:id="rId15" ref="AT3"/>
-    <hyperlink r:id="rId16" ref="H4"/>
-    <hyperlink r:id="rId17" ref="AT4"/>
-    <hyperlink r:id="rId18" ref="H5"/>
-    <hyperlink r:id="rId19" ref="AT5"/>
-    <hyperlink r:id="rId20" ref="H6"/>
-    <hyperlink r:id="rId21" ref="AT6"/>
-    <hyperlink r:id="rId22" ref="AT7"/>
-    <hyperlink r:id="rId23" ref="AT8"/>
-    <hyperlink r:id="rId24" ref="H10"/>
-    <hyperlink r:id="rId25" ref="AT10"/>
-    <hyperlink r:id="rId26" ref="H11"/>
-    <hyperlink r:id="rId27" ref="AT11"/>
-    <hyperlink r:id="rId28" ref="H12"/>
-    <hyperlink r:id="rId29" ref="AT12"/>
-    <hyperlink r:id="rId30" ref="AT13"/>
-    <hyperlink r:id="rId31" ref="AT14"/>
+    <hyperlink ref="G1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="R1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="S1" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="X1" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Y1" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AH1" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AI1" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AK1" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AL1" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AM1" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AN1" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AT1" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H2" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AT2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AT3" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="AT4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="AT5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="AT6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="AT7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="AT8" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="AT10" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H11" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="AT11" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H12" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AT12" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AT13" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="AT14" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
   </hyperlinks>
-  <drawing r:id="rId32"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create updated zone 1 activity
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E43600-D06B-5943-84CA-4C67E742EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="3060" windowWidth="20100" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -47,15 +41,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.spsnational.org/about/governance/zones</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -98,15 +95,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>email1@mail.edu</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">; </t>
     </r>
@@ -114,15 +114,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>email2@mail.edu</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -135,8 +138,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.spsnational.org/about/governance/national-council/nominations-elections</t>
     </r>
@@ -161,8 +165,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>www.spsnational.org/code-conduct</t>
     </r>
@@ -175,8 +180,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.sigmapisigma.org/congress/2022</t>
     </r>
@@ -213,15 +219,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>www.spsnational.org</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> website?</t>
     </r>
@@ -234,15 +243,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>www.spsnational.org</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> website? </t>
     </r>
@@ -258,8 +270,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>www.spsnational.org/about/governance/sps-information-handbook</t>
     </r>
@@ -272,8 +285,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.sigmapisigma.org/sigmapisigma/pion-resources</t>
     </r>
@@ -286,15 +300,18 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.spsnational.org/awards/service</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -302,8 +319,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.sigmapisigma.org/sigmapisigma/awards/outstanding-service</t>
     </r>
@@ -316,8 +334,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>www.spsnational.org/careerstoolbox</t>
     </r>
@@ -345,8 +364,9 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155CC"/>
+        <color rgb="FF1155cc"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://rb.gy/atr9rp</t>
     </r>
@@ -1120,47 +1140,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000ff"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155cc"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1171,7 +1179,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -1183,43 +1198,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="11">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -1246,22 +1279,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1273,131 +1366,158 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1408,1917 +1528,1928 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.83203125" customWidth="1"/>
-    <col min="46" max="46" width="24" customWidth="1"/>
+    <col min="1" max="1" style="8" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="22.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="9" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
     </row>
-    <row r="2" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
-        <v>45448.510231481479</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="1">
+        <v>45448.51023148148</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z2" s="3">
+      <c r="W2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z2" s="6">
         <v>20</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AH2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1" t="s">
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AT2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AU2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
     </row>
-    <row r="3" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
-        <v>45455.846261574072</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="1">
+        <v>45455.84626157407</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="S3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z3" s="3">
+      <c r="W3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z3" s="6">
         <v>30</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="3">
+      <c r="AA3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="6">
         <v>4</v>
       </c>
-      <c r="AH3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AH3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AR3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AS3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AT3" s="5" t="s">
+      <c r="AT3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AU3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AV3" s="1"/>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
     </row>
-    <row r="4" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="1">
         <v>45458.85255787037</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z4" s="3">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z4" s="6">
         <v>150</v>
       </c>
-      <c r="AA4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1" t="s">
+      <c r="AA4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AD4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1" t="s">
+      <c r="AD4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AM4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1" t="s">
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AT4" s="5" t="s">
+      <c r="AT4" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AU4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
-      <c r="AZ4" s="1"/>
-      <c r="BA4" s="1"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
     </row>
-    <row r="5" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
-        <v>45457.865810185183</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="1">
+        <v>45457.86581018518</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="S5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z5" s="3">
+      <c r="W5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="6">
         <v>100</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1" t="s">
+      <c r="AA5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AD5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1" t="s">
+      <c r="AD5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AG5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AH5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AH5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AK5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AK5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AM5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AR5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AS5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AT5" s="5" t="s">
+      <c r="AT5" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AU5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
-      <c r="AX5" s="1"/>
-      <c r="AY5" s="1"/>
-      <c r="AZ5" s="1"/>
-      <c r="BA5" s="1"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
     </row>
-    <row r="6" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="1">
         <v>45455.72483796296</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>1</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="1" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z6" s="3">
+      <c r="W6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z6" s="6">
         <v>14</v>
       </c>
-      <c r="AA6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1" t="s">
+      <c r="AA6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1" t="s">
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AT6" s="4" t="s">
+      <c r="AT6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
-      <c r="AX6" s="1"/>
-      <c r="AY6" s="1"/>
-      <c r="AZ6" s="1"/>
-      <c r="BA6" s="1"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
     </row>
-    <row r="7" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>45457.566967592589</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="1">
+        <v>45457.56696759259</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z7" s="3">
+      <c r="W7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z7" s="6">
         <v>20</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AA7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AC7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AE7" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AF7" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AG7" s="6">
         <v>1</v>
       </c>
-      <c r="AH7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AH7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AJ7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AK7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AK7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="AM7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AR7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AS7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AT7" s="4" t="s">
+      <c r="AT7" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AU7" s="1"/>
-      <c r="AV7" s="1"/>
-      <c r="AW7" s="1"/>
-      <c r="AX7" s="1"/>
-      <c r="AY7" s="1"/>
-      <c r="AZ7" s="1"/>
-      <c r="BA7" s="1"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
     </row>
-    <row r="8" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
-        <v>45457.489664351851</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="1">
+        <v>45457.48966435185</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" s="1" t="s">
+      <c r="S8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="W8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z8" s="3">
+      <c r="W8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="6">
         <v>30</v>
       </c>
-      <c r="AA8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1" t="s">
+      <c r="AA8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="AD8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1" t="s">
+      <c r="AD8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AG8" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="AH8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AH8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO8" s="1"/>
-      <c r="AP8" s="1" t="s">
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="1" t="s">
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AS8" s="1" t="s">
+      <c r="AS8" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="AT8" s="5" t="s">
+      <c r="AT8" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="AU8" s="1" t="s">
+      <c r="AU8" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AV8" s="1"/>
-      <c r="AW8" s="1"/>
-      <c r="AX8" s="1"/>
-      <c r="AY8" s="1"/>
-      <c r="AZ8" s="1"/>
-      <c r="BA8" s="1"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
     </row>
-    <row r="9" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
-        <v>45411.404606481483</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+      <c r="A9" s="1">
+        <v>45411.40460648148</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T9" s="1" t="s">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z9" s="3">
+      <c r="W9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9" s="6">
         <v>20</v>
       </c>
-      <c r="AA9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1" t="s">
+      <c r="AA9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AD9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1" t="s">
+      <c r="AD9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="6">
         <v>1</v>
       </c>
-      <c r="AH9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI9" s="1" t="s">
+      <c r="AH9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ9" s="1" t="s">
+      <c r="AJ9" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AK9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL9" s="1" t="s">
+      <c r="AK9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
+      <c r="AM9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ9" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="1"/>
-      <c r="AZ9" s="1"/>
-      <c r="BA9" s="1"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
     </row>
-    <row r="10" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="1">
         <v>45447.74181712963</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="S10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z10" s="3">
+      <c r="W10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z10" s="6">
         <v>48</v>
       </c>
-      <c r="AA10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1" t="s">
+      <c r="AA10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AD10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1" t="s">
+      <c r="AD10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AG10" s="6">
         <v>5</v>
       </c>
-      <c r="AH10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
+      <c r="AH10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="AR10" s="1" t="s">
+      <c r="AR10" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AS10" s="1" t="s">
+      <c r="AS10" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AT10" s="5" t="s">
+      <c r="AT10" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="AU10" s="1" t="s">
+      <c r="AU10" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-      <c r="AY10" s="1"/>
-      <c r="AZ10" s="1"/>
-      <c r="BA10" s="1"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
     </row>
-    <row r="11" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="1">
         <v>45450.921956018516</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T11" s="1" t="s">
+      <c r="S11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="W11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z11" s="3">
+      <c r="W11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z11" s="6">
         <v>75</v>
       </c>
-      <c r="AA11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AA11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB11" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AD11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1" t="s">
+      <c r="AD11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AG11" s="6">
         <v>1</v>
       </c>
-      <c r="AH11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI11" s="1" t="s">
+      <c r="AH11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL11" s="1" t="s">
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
+      <c r="AM11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="AR11" s="1" t="s">
+      <c r="AR11" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AS11" s="1" t="s">
+      <c r="AS11" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AT11" s="5" t="s">
+      <c r="AT11" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="AU11" s="1" t="s">
+      <c r="AU11" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
-      <c r="AY11" s="1"/>
-      <c r="AZ11" s="1"/>
-      <c r="BA11" s="1"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
     </row>
-    <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
-        <v>45465.165208333332</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+      <c r="A12" s="1">
+        <v>45465.16520833333</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T12" s="1" t="s">
+      <c r="S12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="W12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z12" s="3">
+      <c r="W12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z12" s="6">
         <v>60</v>
       </c>
-      <c r="AA12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AA12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB12" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AC12" s="1" t="s">
+      <c r="AC12" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AD12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE12" s="1" t="s">
+      <c r="AD12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE12" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AF12" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="6">
         <v>2</v>
       </c>
-      <c r="AH12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL12" s="1" t="s">
+      <c r="AH12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO12" s="1"/>
-      <c r="AP12" s="1" t="s">
+      <c r="AM12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AQ12" s="1" t="s">
+      <c r="AQ12" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AR12" s="1" t="s">
+      <c r="AR12" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="AS12" s="1" t="s">
+      <c r="AS12" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AT12" s="4" t="s">
+      <c r="AT12" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="AU12" s="1"/>
-      <c r="AV12" s="1"/>
-      <c r="AW12" s="1"/>
-      <c r="AX12" s="1"/>
-      <c r="AY12" s="1"/>
-      <c r="AZ12" s="1"/>
-      <c r="BA12" s="1"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
     </row>
-    <row r="13" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+      <c r="A13" s="1">
         <v>45454.738020833334</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="6">
         <v>1</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="S13" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="U13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="W13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y13" s="1" t="s">
+      <c r="W13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="6">
         <v>20</v>
       </c>
-      <c r="AA13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1" t="s">
+      <c r="AA13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="AD13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1" t="s">
+      <c r="AD13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="AG13" s="3">
+      <c r="AG13" s="6">
         <v>1</v>
       </c>
-      <c r="AH13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL13" s="1" t="s">
+      <c r="AH13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AM13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ13" s="1" t="s">
+      <c r="AM13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="1" t="s">
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="AT13" s="5" t="s">
+      <c r="AT13" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="AU13" s="1" t="s">
+      <c r="AU13" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="AV13" s="1"/>
-      <c r="AW13" s="1"/>
-      <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
-      <c r="AZ13" s="1"/>
-      <c r="BA13" s="1"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
     </row>
-    <row r="14" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="7">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="1">
         <v>45450.969664351855</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="U14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z14" s="3">
+      <c r="W14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z14" s="6">
         <v>32</v>
       </c>
-      <c r="AA14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AA14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AC14" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AD14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1" t="s">
+      <c r="AD14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="AG14" s="3">
+      <c r="AG14" s="6">
         <v>2</v>
       </c>
-      <c r="AH14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO14" s="1"/>
-      <c r="AP14" s="1" t="s">
+      <c r="AH14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="AQ14" s="1"/>
-      <c r="AR14" s="1"/>
-      <c r="AS14" s="1" t="s">
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AT14" s="5" t="s">
+      <c r="AT14" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="AU14" s="1" t="s">
+      <c r="AU14" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AV14" s="1"/>
-      <c r="AW14" s="1"/>
-      <c r="AX14" s="1"/>
-      <c r="AY14" s="1"/>
-      <c r="AZ14" s="1"/>
-      <c r="BA14" s="1"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="R1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="S1" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="X1" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="Y1" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="AH1" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="AI1" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="AK1" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AL1" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="AM1" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="AN1" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="AT1" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H2" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="AT2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="AT3" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="AT4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="H5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="AT5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="AT6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="AT7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="AT8" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="H10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="AT10" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H11" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="AT11" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H12" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="AT12" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="AT13" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="AT14" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Format target and master files
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7712FF-70C4-5E49-9A17-8D31736BAAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -41,7 +47,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -95,7 +101,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -114,7 +120,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -138,7 +144,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -165,7 +171,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -180,7 +186,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -219,7 +225,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -243,7 +249,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -270,7 +276,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -285,7 +291,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -300,7 +306,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -319,7 +325,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -334,7 +340,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -364,7 +370,7 @@
       <rPr>
         <u/>
         <sz val="10"/>
-        <color rgb="FF1155cc"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -1140,9 +1146,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,14 +1164,27 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000ff"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF1155cc"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1199,46 +1217,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1249,10 +1268,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -1290,71 +1309,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1382,7 +1401,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1405,11 +1424,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1418,13 +1437,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1434,7 +1453,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1443,7 +1462,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1452,7 +1471,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1460,10 +1479,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1528,72 +1547,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="8" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="9" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="25" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="45" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="24" bestFit="1" customWidth="1"/>
+    <col min="47" max="53" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row r="1" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1606,10 +1593,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1742,9 +1729,9 @@
       <c r="AZ1" s="2"/>
       <c r="BA1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row r="2" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>45448.51023148148</v>
+        <v>45448.510231481479</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>47</v>
@@ -1861,9 +1848,9 @@
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row r="3" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>45455.84626157407</v>
+        <v>45455.846261574072</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>64</v>
@@ -1996,7 +1983,7 @@
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row r="4" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45458.85255787037</v>
       </c>
@@ -2125,9 +2112,9 @@
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row r="5" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>45457.86581018518</v>
+        <v>45457.865810185183</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>103</v>
@@ -2266,7 +2253,7 @@
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row r="6" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45455.72483796296</v>
       </c>
@@ -2361,9 +2348,9 @@
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row r="7" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45457.56696759259</v>
+        <v>45457.566967592589</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>137</v>
@@ -2486,9 +2473,9 @@
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row r="8" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45457.48966435185</v>
+        <v>45457.489664351851</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>152</v>
@@ -2623,9 +2610,9 @@
       <c r="AZ8" s="2"/>
       <c r="BA8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row r="9" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45411.40460648148</v>
+        <v>45411.404606481483</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>175</v>
@@ -2752,7 +2739,7 @@
       <c r="AZ9" s="2"/>
       <c r="BA9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row r="10" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45447.74181712963</v>
       </c>
@@ -2891,7 +2878,7 @@
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row r="11" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45450.921956018516</v>
       </c>
@@ -3032,9 +3019,9 @@
       <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row r="12" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45465.16520833333</v>
+        <v>45465.165208333332</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>239</v>
@@ -3175,7 +3162,7 @@
       <c r="AZ12" s="2"/>
       <c r="BA12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row r="13" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45454.738020833334</v>
       </c>
@@ -3310,7 +3297,7 @@
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row r="14" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45450.969664351855</v>
       </c>
@@ -3449,6 +3436,9 @@
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2"/>
     </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Formatting target and master files
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7712FF-70C4-5E49-9A17-8D31736BAAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6318FB-0A9F-894F-B234-517643E3C56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1566,9 +1566,9 @@
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="29.5" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="8" max="8" width="45.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" customWidth="1"/>
     <col min="11" max="13" width="12.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="25" width="12.5" bestFit="1" customWidth="1"/>
@@ -3441,5 +3441,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update base files for testing
Re-testing that updates work on the President name and email columns.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678311B2-AD1C-2340-86ED-8EFA4A528F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E9CE33-9423-D84D-ABC8-73357166DE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3220" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-2720" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1563,7 +1563,7 @@
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.33203125" customWidth="1"/>
@@ -1745,7 +1745,7 @@
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1997,7 +1997,7 @@
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="10" t="s">
         <v>87</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -2126,7 +2126,7 @@
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="10" t="s">
         <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -2267,7 +2267,7 @@
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
         <v>131</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -2364,7 +2364,7 @@
       <c r="D7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="10" t="s">
         <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2487,7 +2487,7 @@
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>154</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -2624,7 +2624,7 @@
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>177</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -2753,7 +2753,7 @@
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>195</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -3035,7 +3035,7 @@
       <c r="D12" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>241</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -3176,7 +3176,7 @@
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="10" t="s">
         <v>261</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -3313,7 +3313,7 @@
       <c r="D14" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="10" t="s">
         <v>283</v>
       </c>
       <c r="F14" s="2" t="s">

</xml_diff>

<commit_message>
Update base files for induction date testing
Basically, I want to end up at the point where the induction date was working but 2 of the schools (Smith and UoMass-Amherst) had wrong date entries.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E9CE33-9423-D84D-ABC8-73357166DE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201F0398-6EF3-F643-A44A-71D485116800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2720" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-3220" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1745,7 +1745,7 @@
       <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1997,7 +1997,7 @@
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -2126,7 +2126,7 @@
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="2" t="s">
         <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -2267,7 +2267,7 @@
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="2" t="s">
         <v>131</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -2364,7 +2364,7 @@
       <c r="D7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="2" t="s">
         <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2487,7 +2487,7 @@
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -2624,7 +2624,7 @@
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="2" t="s">
         <v>177</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -2753,7 +2753,7 @@
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="2" t="s">
         <v>195</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -3035,7 +3035,7 @@
       <c r="D12" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="2" t="s">
         <v>241</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -3176,7 +3176,7 @@
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="2" t="s">
         <v>261</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -3313,7 +3313,7 @@
       <c r="D14" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="2" t="s">
         <v>283</v>
       </c>
       <c r="F14" s="2" t="s">

</xml_diff>

<commit_message>
Debug error in induction date (see description)
In an effort to understand why only 8 out of the 13 entries from the submitted chapters in Zone 1 had their last induction dates updated, I added print statements for debugging to identify the issue. The debugging process revealed significant mismatches, such as Harvard College being incorrectly matched to Hannover College and Smith College to Ithaca College. This is clearly problematic. Two potential solutions come to mind: either completely separate the logic for updating induction dates from the rest of the record updating process or filter the MHS chapters to only include Zone 1 schools. I will start by implementing the former.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C6CAE1-C002-2B42-B991-A04E7F9FA3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC024A5-CA39-3D4A-A928-A1B9732A8BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Decouple induction date update logic
I tested out the new code by ensuring that, first, `update_record` works on correctly updating the SPS president name and email.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC024A5-CA39-3D4A-A928-A1B9732A8BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FD394-B7FB-DB49-9A51-DD99542962A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1739,7 @@
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1993,7 +1993,7 @@
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
@@ -2263,7 +2263,7 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
@@ -2483,7 +2483,7 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
@@ -2620,7 +2620,7 @@
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
@@ -2749,7 +2749,7 @@
       <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="2" t="s">
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
@@ -3307,7 +3307,7 @@
       <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="2" t="s">
         <v>281</v>
       </c>
       <c r="D14" s="2" t="s">

</xml_diff>

<commit_message>
Filter Target df Using Master 4 Induction updates
The issue is that the current school_name is being selected from a wide range of schools listed under the ‘Custom Field Data - Chapter School Name’ column in target_df, derived from the Zone 1 Activity data. This broad selection introduces many schools that should not be the focus. Instead, we need to concentrate on the schools that actually submitted their chapter reports this year, which are listed in master_df from the ‘24 Reports Zone 1’ file. We then compare these specific schools against those in induction_df from the ‘MHS Chapters’ file. If a last induction date is found in ‘MHS Chapters’, we update target_df with that induction date. This approach ensures we only focus on the schools that submitted their chapter reports, avoiding the inclusion of unrelated schools from Zone 1.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FD394-B7FB-DB49-9A51-DD99542962A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B271962-7592-DF44-9824-A3A788EBAD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1739,7 @@
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1993,7 +1993,7 @@
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
@@ -2263,7 +2263,7 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
@@ -2358,7 +2358,7 @@
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2483,7 +2483,7 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
@@ -2620,7 +2620,7 @@
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
@@ -2749,7 +2749,7 @@
       <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
@@ -3029,7 +3029,7 @@
       <c r="B12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>240</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3172,7 +3172,7 @@
       <c r="B13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
@@ -3307,7 +3307,7 @@
       <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>281</v>
       </c>
       <c r="D14" s="2" t="s">

</xml_diff>

<commit_message>
FINALLY handle last induction date update logic
In my effort to focus solely on updating the schools that have recently submitted their chapter reports, I used the following logic. While this approach has worked successfully for Zone 1, a potential issue may arise where school names in both files are similar but not an exact match, a problem I encountered early on and resolved using fuzzy matching. Since this hasn’t posed a problem yet and I need to update the rest of the columns with limited time remaining, I will keep this line as it is. If it causes issues later or once I have completed everything else, I will address this potential bug at the end.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B271962-7592-DF44-9824-A3A788EBAD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C25D40E-FCB3-9548-8089-EA310BC518C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1739,7 @@
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1993,7 +1993,7 @@
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
@@ -2263,7 +2263,7 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
@@ -2358,7 +2358,7 @@
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2483,7 +2483,7 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
@@ -2620,7 +2620,7 @@
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
@@ -2749,7 +2749,7 @@
       <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="2" t="s">
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
@@ -3029,7 +3029,7 @@
       <c r="B12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="2" t="s">
         <v>240</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3172,7 +3172,7 @@
       <c r="B13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="2" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
@@ -3307,7 +3307,7 @@
       <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="2" t="s">
         <v>281</v>
       </c>
       <c r="D14" s="2" t="s">

</xml_diff>

<commit_message>
Begin testing for chapter report year
I received an error, "TypeError: argument of type 'int' is not iterable" but I wanted to commit everything first as a first step into working in this branch.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C25D40E-FCB3-9548-8089-EA310BC518C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87CF134-04E0-2C46-BEC4-F1D0CB188401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
   </sheetPr>
   <dimension ref="A1:BA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Incorporate fuzzy matching (not yet correct)
I incorporated fuzzy matching, and the chapter report (year) column was updated more accurately than before. However, an issue arose where ‘Harvard College’ from ‘24 Reports Zone 1’ had a higher similarity score with ‘Marlboro College’ (score of 71) than with ‘Harvard University’ in ‘Zone 1 Activity’ (score of 42). This led to the chapter report (year) column for ‘Marlboro College’ being updated instead of ‘Harvard University’s’.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87CF134-04E0-2C46-BEC4-F1D0CB188401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE1013A-7A09-6D47-AB89-47E285561AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1739,7 @@
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1993,7 +1993,7 @@
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
@@ -2263,7 +2263,7 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
@@ -2358,7 +2358,7 @@
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2483,7 +2483,7 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
@@ -2620,7 +2620,7 @@
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
@@ -2749,7 +2749,7 @@
       <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
@@ -2888,7 +2888,7 @@
       <c r="B11" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>217</v>
       </c>
       <c r="D11" s="2"/>
@@ -3029,7 +3029,7 @@
       <c r="B12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>240</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3172,7 +3172,7 @@
       <c r="B13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
@@ -3307,7 +3307,7 @@
       <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>281</v>
       </c>
       <c r="D14" s="2" t="s">

</xml_diff>

<commit_message>
First attempt at testing
I have included just 'Harvard College ', 'University of Massachusetts Amherst', 'Fairfield University'. I am getting some fails and I am refining my testing.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE1013A-7A09-6D47-AB89-47E285561AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D14B6-54C5-D142-BA82-5F88B96F194C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1147,7 +1147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1188,6 +1188,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1213,10 +1221,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1246,8 +1255,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1554,7 +1567,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1752,7 @@
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1748,7 +1761,7 @@
       <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="6">
@@ -1993,7 +2006,7 @@
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="2"/>
@@ -2122,7 +2135,7 @@
       <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="2"/>
@@ -2263,7 +2276,7 @@
       <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="2"/>
@@ -2358,7 +2371,7 @@
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2483,7 +2496,7 @@
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="2"/>
@@ -2620,7 +2633,7 @@
       <c r="B9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="2"/>
@@ -2749,7 +2762,7 @@
       <c r="B10" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="2" t="s">
         <v>194</v>
       </c>
       <c r="D10" s="2"/>
@@ -2888,7 +2901,7 @@
       <c r="B11" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="2" t="s">
         <v>217</v>
       </c>
       <c r="D11" s="2"/>
@@ -3029,7 +3042,7 @@
       <c r="B12" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="2" t="s">
         <v>240</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -3172,7 +3185,7 @@
       <c r="B13" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="2" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="2"/>
@@ -3307,7 +3320,7 @@
       <c r="B14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="2" t="s">
         <v>281</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3443,6 +3456,9 @@
       <c r="F18" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{2EACCA7B-BF21-0C4B-838D-7345D70FE99A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
(fail) Trimming School Names 4 Easier Comparisons
It failed so I am in the process of debugging.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463812B2-6F8B-4E42-B06E-6048CC14F66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0392E91-9CC5-074C-8D64-C7A773CDDA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1567,7 +1567,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
(success) Trimming Sch Names 4 Easier Comparisons.
It finally worked. The key was to delete the line `# school_name = school_name.strip() # Trim whitespace from the school name` which altered the trimming somehow, I don't know how.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0392E91-9CC5-074C-8D64-C7A773CDDA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8343B07-B9BD-0341-BA07-E224DF16E49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1567,7 +1567,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add sch name trimming in `update_chapter_reports`
It works. I checked the result Excel file against all 14 schools which submitted their chapter reports.
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8343B07-B9BD-0341-BA07-E224DF16E49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F95079-4B20-1F43-BBE9-DC2B87AADB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1567,7 +1567,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1575,7 @@
     <col min="1" max="1" width="16" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
     <col min="5" max="5" width="47.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="9" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Ensure curr yr is added as int when no yr present
</commit_message>
<xml_diff>
--- a/24 Reports Zone 1.xlsx
+++ b/24 Reports Zone 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F95079-4B20-1F43-BBE9-DC2B87AADB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A279F8-A99F-4848-828B-4A6A25922947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1567,7 +1567,7 @@
   <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>